<commit_message>
Subject text wrap added
</commit_message>
<xml_diff>
--- a/Sample-Data/Student.xlsx
+++ b/Sample-Data/Student.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT\student-report-visualizer\Sample-Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{883E73ED-D081-42C4-9F0F-7B2F2341F2B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24009D87-230A-493E-938F-8D9C7B9641C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{254E0297-E6FD-4620-A106-9A2866B481C4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
   <si>
     <t>Name</t>
   </si>
@@ -63,28 +63,13 @@
     <t>Sub-22</t>
   </si>
   <si>
-    <t>Sub-18</t>
-  </si>
-  <si>
     <t>Sub-19</t>
   </si>
   <si>
-    <t>Sub-16</t>
-  </si>
-  <si>
     <t>Sub-25</t>
   </si>
   <si>
-    <t>Sub-15</t>
-  </si>
-  <si>
     <t>Sub-28</t>
-  </si>
-  <si>
-    <t>Sub-29</t>
-  </si>
-  <si>
-    <t>Sub-30</t>
   </si>
 </sst>
 </file>
@@ -442,10 +427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93D551B0-87FA-45FA-BAD4-739FB85B2487}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18:D21"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -528,10 +513,10 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D6">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -573,7 +558,7 @@
         <v>6</v>
       </c>
       <c r="D9">
-        <v>84</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -584,10 +569,10 @@
         <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D10">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -595,13 +580,13 @@
         <v>4</v>
       </c>
       <c r="B11">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D11">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -609,139 +594,13 @@
         <v>4</v>
       </c>
       <c r="B12">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D12">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13">
-        <v>10</v>
-      </c>
-      <c r="C13" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14">
-        <v>7</v>
-      </c>
-      <c r="C14" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15">
-        <v>7</v>
-      </c>
-      <c r="C15" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16">
-        <v>10</v>
-      </c>
-      <c r="C16" t="s">
-        <v>16</v>
-      </c>
-      <c r="D16">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17">
-        <v>10</v>
-      </c>
-      <c r="C17" t="s">
-        <v>15</v>
-      </c>
-      <c r="D17">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18">
-        <v>10</v>
-      </c>
-      <c r="C18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D18">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>4</v>
-      </c>
-      <c r="B19">
-        <v>12</v>
-      </c>
-      <c r="C19" t="s">
-        <v>17</v>
-      </c>
-      <c r="D19">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>4</v>
-      </c>
-      <c r="B20">
-        <v>12</v>
-      </c>
-      <c r="C20" t="s">
-        <v>18</v>
-      </c>
-      <c r="D20">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>4</v>
-      </c>
-      <c r="B21">
-        <v>12</v>
-      </c>
-      <c r="C21" t="s">
-        <v>19</v>
-      </c>
-      <c r="D21">
-        <v>66</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
On Slider Move event Updated
</commit_message>
<xml_diff>
--- a/Sample-Data/Student.xlsx
+++ b/Sample-Data/Student.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT\student-report-visualizer\Sample-Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24009D87-230A-493E-938F-8D9C7B9641C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40D7CE7F-0B2D-4233-9F63-A9AD9BEB7B40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{254E0297-E6FD-4620-A106-9A2866B481C4}"/>
   </bookViews>
@@ -430,7 +430,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="A13" sqref="A13:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>